<commit_message>
updating with April invoicing
</commit_message>
<xml_diff>
--- a/2024.04 Invoicing/ethylene_oxide_invoice_April_2024.xlsx
+++ b/2024.04 Invoicing/ethylene_oxide_invoice_April_2024.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,6 +455,60 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>CL001</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Johnson</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="D2" t="n">
+        <v>13.33</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>CL007</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Shah/Rieke</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1.33</v>
+      </c>
+      <c r="D3" t="n">
+        <v>53.33</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>CL010</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Silverton</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="D4" t="n">
+        <v>13.33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>